<commit_message>
Tried to fix most stuff
</commit_message>
<xml_diff>
--- a/database_excel_files/Suggestion.xlsx
+++ b/database_excel_files/Suggestion.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/c220096_e_ntu_edu_sg/Documents/Desktop/SC2002_Lab_Project-YQ1/database_excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0xd1rac\Code\SC2002_Lab_Project\database_excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2476118D-4727-4B2F-B46F-5A0DCF7786B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64F09261-968C-4BD5-AF86-FA1606950A1C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DBBA08-E993-4B82-AC7C-829D5160C550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -33,13 +33,116 @@
     <t>isProcessed</t>
   </si>
   <si>
-    <t>suggestion_str</t>
+    <t>campId</t>
+  </si>
+  <si>
+    <t>newCampName</t>
+  </si>
+  <si>
+    <t>newCampIsVisible</t>
+  </si>
+  <si>
+    <t>newCampEndDate</t>
+  </si>
+  <si>
+    <t>newCampStartDate</t>
+  </si>
+  <si>
+    <t>newRegClosingDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newLocation </t>
+  </si>
+  <si>
+    <t>newTotalSlots</t>
+  </si>
+  <si>
+    <t>newCampCommitteeSlots</t>
+  </si>
+  <si>
+    <t>newDescription</t>
+  </si>
+  <si>
+    <t>isApproved</t>
+  </si>
+  <si>
+    <t>5f1b0de2ae8d47b38a1d1f1e1d4601c2</t>
+  </si>
+  <si>
+    <t>campId1</t>
+  </si>
+  <si>
+    <t>New Camp One</t>
+  </si>
+  <si>
+    <t>2023-08-01</t>
+  </si>
+  <si>
+    <t>2023-08-15</t>
+  </si>
+  <si>
+    <t>2023-07-15</t>
+  </si>
+  <si>
+    <t>New Location One</t>
+  </si>
+  <si>
+    <t>New Description One</t>
+  </si>
+  <si>
+    <t>9f4e2a7f0f924325a491f8f11c21f419</t>
+  </si>
+  <si>
+    <t>campId2</t>
+  </si>
+  <si>
+    <t>New Camp Two</t>
+  </si>
+  <si>
+    <t>New Location Two</t>
+  </si>
+  <si>
+    <t>New Description Two</t>
+  </si>
+  <si>
+    <t>0c46add4f58c4a99917d58433720f7be</t>
+  </si>
+  <si>
+    <t>campId3</t>
+  </si>
+  <si>
+    <t>New Camp Three</t>
+  </si>
+  <si>
+    <t>New Location Three</t>
+  </si>
+  <si>
+    <t>New Description Three</t>
+  </si>
+  <si>
+    <t>updatedCampId</t>
+  </si>
+  <si>
+    <t>Updated Camp</t>
+  </si>
+  <si>
+    <t>2023-09-01</t>
+  </si>
+  <si>
+    <t>2023-09-15</t>
+  </si>
+  <si>
+    <t>Updated Location</t>
+  </si>
+  <si>
+    <t>udpated descrition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,29 +454,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="2" max="3" customWidth="true" width="26.85546875"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125"/>
+    <col min="5" max="5" customWidth="true" width="22.42578125"/>
+    <col min="6" max="6" customWidth="true" width="21.85546875"/>
+    <col min="7" max="7" customWidth="true" width="26.0"/>
+    <col min="8" max="8" customWidth="true" width="20.42578125"/>
+    <col min="9" max="9" customWidth="true" width="26.28515625"/>
+    <col min="10" max="10" customWidth="true" width="18.5703125"/>
+    <col min="11" max="11" customWidth="true" width="19.42578125"/>
+    <col min="12" max="12" customWidth="true" width="26.5703125"/>
+    <col min="13" max="13" customWidth="true" width="18.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B2" t="b" s="0">
         <v>1</v>
+      </c>
+      <c r="C2" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="F2" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="K2" t="n" s="0">
+        <v>80.0</v>
+      </c>
+      <c r="L2" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B3" t="b" s="0">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="F3" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="K3" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="L3" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>